<commit_message>
Fixed Publisher column - needed space
</commit_message>
<xml_diff>
--- a/data/doaj-article-sample.xlsx
+++ b/data/doaj-article-sample.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10978" uniqueCount="5935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10978" uniqueCount="5936">
   <si>
     <t>Title</t>
   </si>
@@ -17832,6 +17832,9 @@
   </si>
   <si>
     <t>International Union of Crystallography; Chester, England</t>
+  </si>
+  <si>
+    <t>MDPI AG  ; Basel, Switzerland</t>
   </si>
 </sst>
 </file>
@@ -18148,8 +18151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19260,7 +19263,7 @@
         <v>218</v>
       </c>
       <c r="I32" t="s">
-        <v>5929</v>
+        <v>5935</v>
       </c>
       <c r="J32" t="s">
         <v>219</v>
@@ -19295,7 +19298,7 @@
         <v>225</v>
       </c>
       <c r="I33" t="s">
-        <v>5929</v>
+        <v>5935</v>
       </c>
       <c r="J33" t="s">
         <v>226</v>
@@ -19709,7 +19712,7 @@
         <v>305</v>
       </c>
       <c r="I45" t="s">
-        <v>5929</v>
+        <v>5935</v>
       </c>
       <c r="J45" t="s">
         <v>306</v>

</xml_diff>